<commit_message>
Add tasks for team
Add tasks for team
</commit_message>
<xml_diff>
--- a/Lab3-Tasks.xlsx
+++ b/Lab3-Tasks.xlsx
@@ -9,17 +9,18 @@
   <sheets>
     <sheet name="Lab3-Tasks" sheetId="5" r:id="rId1"/>
     <sheet name="Lab3-CheckList" sheetId="7" r:id="rId2"/>
+    <sheet name="TokenCode" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Lab3-Tasks'!$A$1:$H$6</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Lab3-Tasks'!$F$1:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Lab3-Tasks'!$A$1:$E$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Lab3-Tasks'!$D$1:$E$6</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="131">
   <si>
     <t>Comment</t>
   </si>
@@ -33,30 +34,9 @@
     <t>% Completed</t>
   </si>
   <si>
-    <t>Function name</t>
-  </si>
-  <si>
-    <t>Pseudocode required?</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>Test code required?</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Function description</t>
-  </si>
-  <si>
-    <t>main function</t>
-  </si>
-  <si>
     <t>pseudocode for each function</t>
   </si>
   <si>
@@ -121,13 +101,325 @@
   </si>
   <si>
     <t>Created but empty</t>
+  </si>
+  <si>
+    <t>NO_TOKEN</t>
+  </si>
+  <si>
+    <t>IDENTIFIER</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>UPARROW</t>
+  </si>
+  <si>
+    <t>STAR</t>
+  </si>
+  <si>
+    <t>LPAREN</t>
+  </si>
+  <si>
+    <t>RPAREN</t>
+  </si>
+  <si>
+    <t>MINUS</t>
+  </si>
+  <si>
+    <t>PLUS</t>
+  </si>
+  <si>
+    <t>EQUAL</t>
+  </si>
+  <si>
+    <t>LBRACKET</t>
+  </si>
+  <si>
+    <t>RBRACKET</t>
+  </si>
+  <si>
+    <t>COLON</t>
+  </si>
+  <si>
+    <t>SEMICOLON</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>COMMA</t>
+  </si>
+  <si>
+    <t>PERIOD</t>
+  </si>
+  <si>
+    <t>SLASH</t>
+  </si>
+  <si>
+    <t>COLONEQUAL</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>DOTDOT</t>
+  </si>
+  <si>
+    <t>END_OF_FILE</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>ARRAY</t>
+  </si>
+  <si>
+    <t>BEGIN</t>
+  </si>
+  <si>
+    <t>CASE</t>
+  </si>
+  <si>
+    <t>CONST</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>DOWNTO</t>
+  </si>
+  <si>
+    <t>ELSE</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>FFILE</t>
+  </si>
+  <si>
+    <t>FOR</t>
+  </si>
+  <si>
+    <t>FUNCTION</t>
+  </si>
+  <si>
+    <t>GOTO</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>LABEL</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>NIL</t>
+  </si>
+  <si>
+    <t>NOT</t>
+  </si>
+  <si>
+    <t>OF</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PACKED</t>
+  </si>
+  <si>
+    <t>PROCEDURE</t>
+  </si>
+  <si>
+    <t>PROGRAM</t>
+  </si>
+  <si>
+    <t>RECORD</t>
+  </si>
+  <si>
+    <t>REPEAT</t>
+  </si>
+  <si>
+    <t>SET</t>
+  </si>
+  <si>
+    <t>THEN</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>UNTIL</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>WHILE</t>
+  </si>
+  <si>
+    <t>WITH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTEGER_LIT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">REAL_LIT </t>
+  </si>
+  <si>
+    <t>STRING_LIT</t>
+  </si>
+  <si>
+    <t>Token Code</t>
+  </si>
+  <si>
+    <t>Token Type</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Task description</t>
+  </si>
+  <si>
+    <t>Implement function static ??? get_char(???);</t>
+  </si>
+  <si>
+    <t>Implement function static ??? skip_comment(???);</t>
+  </si>
+  <si>
+    <t>Implement function static ??? skip_blanks(???);</t>
+  </si>
+  <si>
+    <t>Implement function static ??? get_word(???);</t>
+  </si>
+  <si>
+    <t>Implement function static ??? get_number(???);</t>
+  </si>
+  <si>
+    <t>Implement function static ??? get_string(???);</t>
+  </si>
+  <si>
+    <t>Implement function static ??? get_special(???);</t>
+  </si>
+  <si>
+    <t>Implement function static ??? downshift_word(???);</t>
+  </si>
+  <si>
+    <t>Implement function static BOOLEAN is_reserved_word(???);</t>
+  </si>
+  <si>
+    <t>Write pseudocode for function static ??? get_char(???);</t>
+  </si>
+  <si>
+    <t>Write pseudocode for function static ??? skip_comment(???);</t>
+  </si>
+  <si>
+    <t>Write pseudocode for function static ??? skip_blanks(???);</t>
+  </si>
+  <si>
+    <t>Write pseudocode for function static ??? get_word(???);</t>
+  </si>
+  <si>
+    <t>Write pseudocode for function static ??? get_number(???);</t>
+  </si>
+  <si>
+    <t>Write pseudocode for function static ??? get_string(???);</t>
+  </si>
+  <si>
+    <t>Write pseudocode for function static ??? get_special(???);</t>
+  </si>
+  <si>
+    <t>Write pseudocode for function static ??? downshift_word(???);</t>
+  </si>
+  <si>
+    <t>Write pseudocode for function static BOOLEAN is_reserved_word(???);</t>
+  </si>
+  <si>
+    <t>Write functional test code for function static ??? get_char(???);</t>
+  </si>
+  <si>
+    <t>Write functional test code for function static ??? skip_comment(???);</t>
+  </si>
+  <si>
+    <t>Write functional test code for function static ??? skip_blanks(???);</t>
+  </si>
+  <si>
+    <t>Write functional test code for function static ??? get_word(???);</t>
+  </si>
+  <si>
+    <t>Write functional test code for function static ??? get_number(???);</t>
+  </si>
+  <si>
+    <t>Write functional test code for function static ??? get_string(???);</t>
+  </si>
+  <si>
+    <t>Write functional test code for function static ??? get_special(???);</t>
+  </si>
+  <si>
+    <t>Write functional test code for function static ??? downshift_word(???);</t>
+  </si>
+  <si>
+    <t>Write functional test code for function static BOOLEAN is_reserved_word(???);</t>
+  </si>
+  <si>
+    <t>Write system test code for function main</t>
+  </si>
+  <si>
+    <t>Create empty template doc for Pseudocode-Design</t>
+  </si>
+  <si>
+    <t>Create doc for Team-Contribution-Assessment</t>
+  </si>
+  <si>
+    <t>Create empty template doc for Solution-Document</t>
+  </si>
+  <si>
+    <t>Create empty template doc for Change-History</t>
+  </si>
+  <si>
+    <t>Create empty template for Makefile</t>
+  </si>
+  <si>
+    <t>Create empty template doc for Functional-Test-Table</t>
+  </si>
+  <si>
+    <t>Create empty template doc for System-Test-Table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,8 +440,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +478,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,6 +557,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,11 +864,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,145 +876,565 @@
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.7109375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.42578125" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C2" s="9">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="D2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="B4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="B6" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="B8" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="9">
+        <v>1</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -708,7 +1447,8 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,115 +1461,466 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B63"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="15" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A62">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Check in makefile and code
</commit_message>
<xml_diff>
--- a/Lab3-Tasks.xlsx
+++ b/Lab3-Tasks.xlsx
@@ -571,7 +571,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1102,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Final check in before submit
</commit_message>
<xml_diff>
--- a/Lab3-Tasks.xlsx
+++ b/Lab3-Tasks.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Lab3-Tasks" sheetId="5" r:id="rId1"/>
+    <sheet name="Lab3 Tasks" sheetId="5" r:id="rId1"/>
+    <sheet name="Functional Test" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Lab3-Tasks'!$A$1:$E$31</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Lab3-Tasks'!$D$1:$E$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Functional Test'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Lab3 Tasks'!$A$1:$E$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Lab3 Tasks'!$D$1:$E$6</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="73">
   <si>
     <t>Comment</t>
   </si>
@@ -141,13 +143,124 @@
   </si>
   <si>
     <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Test Procedure</t>
+  </si>
+  <si>
+    <t>Test Case #</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Required Inputs</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Test Purpose</t>
+  </si>
+  <si>
+    <t>writeln;</t>
+  </si>
+  <si>
+    <t>11:  writeln;
+     &gt;&gt; &lt;IDENTIFIER&gt;     writeln
+     &gt;&gt; ;                ;</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>root := 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26:      root := 1;
+     &gt;&gt; &lt;IDENTIFIER&gt;     root
+     &gt;&gt; :=               :=
+     &gt;&gt; &lt;NUMBER&gt;         1
+     &gt;&gt; ;                ;
+</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>CONST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3: CONST
+     &gt;&gt; CONST            const</t>
+  </si>
+  <si>
+    <t>Assert that the require input is present in input file NEWTON.PAS at line 11</t>
+  </si>
+  <si>
+    <t>Assert that the require input is present in input file NEWTON.PAS at line 26</t>
+  </si>
+  <si>
+    <t>Assert that the require input is present in input file NEWTON.PAS at line  3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  13:  read(number);
+     &gt;&gt; &lt;IDENTIFIER&gt;     read
+     &gt;&gt; (                (
+     &gt;&gt; &lt;IDENTIFIER&gt;     number
+     &gt;&gt; )                )
+     &gt;&gt; ;                ;</t>
+  </si>
+  <si>
+    <t>To test a special character token - parentensis</t>
+  </si>
+  <si>
+    <t>read(number);</t>
+  </si>
+  <si>
+    <t>Assert that the require input is present in input file NEWTON.PAS at line  13</t>
+  </si>
+  <si>
+    <t>To test a Reserve word (Key word) token - CONST</t>
+  </si>
+  <si>
+    <t>To test a Number token - 1</t>
+  </si>
+  <si>
+    <t>To test an Identifier token - writeln</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  35: END.
+     &gt;&gt; END              end
+     &gt;&gt; .                .</t>
+  </si>
+  <si>
+    <t>END.</t>
+  </si>
+  <si>
+    <t>To test a special character token - the period (.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,8 +287,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,8 +334,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -230,11 +364,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -294,6 +443,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -599,9 +761,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,4 +1289,168 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="15" style="23" customWidth="1"/>
+    <col min="5" max="6" width="29.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>